<commit_message>
Final upload of V1 of test document
</commit_message>
<xml_diff>
--- a/MedACRTestingSetAndResults/ACR Test Document  V1.xlsx
+++ b/MedACRTestingSetAndResults/ACR Test Document  V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hazen-ScottishACR-Fork\MedACRTestingSetAndResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD8CACB-5D40-457C-8B27-9FBDAAE107F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68132F60-A921-487C-A036-7CE22422E4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB94AA00-146E-4F69-A819-9104D1118357}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{FB94AA00-146E-4F69-A819-9104D1118357}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Data" sheetId="1" r:id="rId1"/>
@@ -250,9 +250,6 @@
     <t>Spatial Resoloution Contrast Response Manual</t>
   </si>
   <si>
-    <t>b0a868e</t>
-  </si>
-  <si>
     <t>Unclear Peaks and Troughs</t>
   </si>
   <si>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>Raig Cor T1 SE'!A1</t>
+  </si>
+  <si>
+    <t>b1a449d</t>
   </si>
 </sst>
 </file>
@@ -958,7 +958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1068,6 +1068,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1732,7 +1735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11E31CE-8653-4894-8E4F-D4DEA5E43A27}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1773,10 +1776,10 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1790,7 +1793,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>58</v>
@@ -1807,10 +1810,10 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1824,10 +1827,10 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,10 +1844,10 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,10 +1861,10 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1875,10 +1878,10 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1907,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA0AF14-82B7-4E02-914B-3F448BA33919}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,13 +1929,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -1956,11 +1959,11 @@
       <c r="M2" s="57"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="58"/>
@@ -1977,7 +1980,7 @@
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="68" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2659,7 +2662,7 @@
         <v>PASS</v>
       </c>
       <c r="H33" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33" s="49"/>
       <c r="J33" s="49"/>
@@ -2688,7 +2691,7 @@
         <v>PASS</v>
       </c>
       <c r="H34" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I34" s="49"/>
       <c r="J34" s="49"/>
@@ -2744,7 +2747,7 @@
         <v>PASS</v>
       </c>
       <c r="H36" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I36" s="49"/>
       <c r="J36" s="49"/>
@@ -2827,7 +2830,7 @@
         <v>PASS</v>
       </c>
       <c r="H39" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I39" s="49"/>
       <c r="J39" s="49"/>
@@ -2880,8 +2883,11 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://github.com/NHSH-MRI-Physics/Hazen-ScottishACR-Fork/commit/b1a449d7c53f9983bb2e519d0d39b4f64e521758" xr:uid="{8F91B50F-F2A8-4AE9-9F3E-E019D7B3E24C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2890,7 +2896,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2908,13 +2914,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -2941,8 +2947,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="58"/>
@@ -2984,7 +2990,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3854,8 +3860,11 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://github.com/NHSH-MRI-Physics/Hazen-ScottishACR-Fork/commit/b1a449d7c53f9983bb2e519d0d39b4f64e521758" xr:uid="{2D478DC8-80A8-4930-A915-DB34ED49A88E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3863,8 +3872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680AEDF1-8AC6-42DA-933A-EFE13CB6E68C}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,13 +3891,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -3915,8 +3924,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="64"/>
@@ -3958,7 +3967,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3976,7 +3985,7 @@
         <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4828,8 +4837,11 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://github.com/NHSH-MRI-Physics/Hazen-ScottishACR-Fork/commit/b1a449d7c53f9983bb2e519d0d39b4f64e521758" xr:uid="{F3EE1F87-DECD-4BBB-B618-2D984C5FECC7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4837,8 +4849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8582CA64-840D-4D3C-A94A-D21D51863C48}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4856,13 +4868,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -4889,8 +4901,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="64"/>
@@ -4932,7 +4944,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -5802,8 +5814,11 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://github.com/NHSH-MRI-Physics/Hazen-ScottishACR-Fork/commit/b1a449d7c53f9983bb2e519d0d39b4f64e521758" xr:uid="{4C64D972-803D-4647-9573-C31D8CD275C3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5812,7 +5827,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5830,13 +5845,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -5863,8 +5878,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="64"/>
@@ -5906,7 +5921,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -6776,8 +6791,11 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://github.com/NHSH-MRI-Physics/Hazen-ScottishACR-Fork/commit/b1a449d7c53f9983bb2e519d0d39b4f64e521758" xr:uid="{5CDAF4F3-24F6-4B87-9194-BB8058171F0B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6785,8 +6803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AEC8280-D452-469E-AA20-08D428679600}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6804,13 +6822,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -6837,8 +6855,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="64"/>
@@ -6880,7 +6898,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -7750,8 +7768,11 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://github.com/NHSH-MRI-Physics/Hazen-ScottishACR-Fork/commit/b1a449d7c53f9983bb2e519d0d39b4f64e521758" xr:uid="{E290C126-F8CF-44EC-BC06-742F8010BCA4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7759,8 +7780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626DC2B3-277F-4CC8-B025-80F1E465D1E0}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7778,13 +7799,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="54"/>
       <c r="G1" s="54"/>
@@ -7811,8 +7832,8 @@
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>68</v>
+      <c r="B3" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="64"/>
@@ -7854,7 +7875,7 @@
         <v>24</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -8724,8 +8745,11 @@
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://github.com/NHSH-MRI-Physics/Hazen-ScottishACR-Fork/commit/b1a449d7c53f9983bb2e519d0d39b4f64e521758" xr:uid="{B720A8CD-4416-45DA-8F94-C8890B359398}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>